<commit_message>
Added models and a base template
</commit_message>
<xml_diff>
--- a/Design_documents/UWEFlix_Data_Dictionary_final.xlsx
+++ b/Design_documents/UWEFlix_Data_Dictionary_final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26216"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobmoran/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\UWEflix_group\Design_documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B5D6D13-AA9F-4C81-B722-AA0EE6FF6358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED7FFC6C-57A7-4193-9615-7E07FAC463DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="22960" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="4155" yWindow="2295" windowWidth="21600" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -656,7 +656,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -786,7 +786,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -814,6 +814,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -826,19 +836,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1155,11 +1152,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="H70" sqref="B70:H70"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
@@ -1170,13 +1167,13 @@
     <col min="8" max="8" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8">
-      <c r="E2" s="17" t="s">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="17"/>
-    </row>
-    <row r="3" spans="2:8">
+      <c r="F2" s="18"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E3" s="8" t="s">
         <v>1</v>
       </c>
@@ -1184,7 +1181,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:8">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E4" s="8" t="s">
         <v>3</v>
       </c>
@@ -1192,22 +1189,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:8">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E5" s="10"/>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B6" s="13" t="s">
+    <row r="6" spans="2:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-    </row>
-    <row r="7" spans="2:8" s="1" customFormat="1">
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+    </row>
+    <row r="7" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1230,7 +1227,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:8">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
@@ -1251,7 +1248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:8">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
@@ -1272,7 +1269,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="2:8">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
@@ -1293,7 +1290,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="2:8">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
@@ -1314,21 +1311,21 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="2:8">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C12" s="12"/>
     </row>
-    <row r="13" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B13" s="13" t="s">
+    <row r="13" spans="2:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-    </row>
-    <row r="14" spans="2:8" s="1" customFormat="1">
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+    </row>
+    <row r="14" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>6</v>
       </c>
@@ -1351,7 +1348,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="2:8">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>29</v>
       </c>
@@ -1372,7 +1369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:8">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>17</v>
       </c>
@@ -1393,7 +1390,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>22</v>
       </c>
@@ -1414,7 +1411,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>25</v>
       </c>
@@ -1435,23 +1432,23 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="50.1" customHeight="1">
-      <c r="B20" s="13" t="s">
+    <row r="20" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-    </row>
-    <row r="21" spans="1:8" s="1" customFormat="1">
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+    </row>
+    <row r="21" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>6</v>
       </c>
@@ -1474,7 +1471,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>36</v>
       </c>
@@ -1495,7 +1492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>39</v>
       </c>
@@ -1516,7 +1513,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>42</v>
       </c>
@@ -1537,7 +1534,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>10</v>
       </c>
@@ -1558,18 +1555,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="50.1" customHeight="1">
-      <c r="B27" s="13" t="s">
+    <row r="27" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-    </row>
-    <row r="28" spans="1:8" s="1" customFormat="1">
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+    </row>
+    <row r="28" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>6</v>
       </c>
@@ -1592,7 +1589,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>48</v>
       </c>
@@ -1613,7 +1610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>51</v>
       </c>
@@ -1632,18 +1629,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="50.1" customHeight="1">
-      <c r="B32" s="13" t="s">
+    <row r="32" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-    </row>
-    <row r="33" spans="2:8" s="1" customFormat="1">
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+    </row>
+    <row r="33" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>6</v>
       </c>
@@ -1666,7 +1663,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="2:8">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>54</v>
       </c>
@@ -1687,7 +1684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:8">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
         <v>36</v>
       </c>
@@ -1708,7 +1705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="2:8">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
         <v>48</v>
       </c>
@@ -1729,7 +1726,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="2:8">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
         <v>58</v>
       </c>
@@ -1746,7 +1743,7 @@
       </c>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="2:8">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>62</v>
       </c>
@@ -1767,7 +1764,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="2:8">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
         <v>66</v>
       </c>
@@ -1788,18 +1785,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="2:8" ht="50.1" customHeight="1">
-      <c r="B42" s="13" t="s">
+    <row r="42" spans="2:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-    </row>
-    <row r="43" spans="2:8" s="1" customFormat="1">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+    </row>
+    <row r="43" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>6</v>
       </c>
@@ -1822,14 +1819,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="2:8" s="1" customFormat="1">
-      <c r="B44" s="18" t="s">
+    <row r="44" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C44" s="18" t="s">
+      <c r="C44" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D44" s="19" t="s">
+      <c r="D44" s="13" t="s">
         <v>49</v>
       </c>
       <c r="E44" s="2"/>
@@ -1839,11 +1836,11 @@
       <c r="G44" s="2">
         <v>1</v>
       </c>
-      <c r="H44" s="19" t="s">
+      <c r="H44" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:8">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
         <v>72</v>
       </c>
@@ -1864,7 +1861,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="2:8">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
         <v>75</v>
       </c>
@@ -1885,7 +1882,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="2:8">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
         <v>77</v>
       </c>
@@ -1906,7 +1903,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="2:8">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
         <v>79</v>
       </c>
@@ -1927,29 +1924,29 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="2:9">
-      <c r="B49" s="20" t="s">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B49" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="C49" s="20" t="s">
+      <c r="C49" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D49" s="20" t="s">
+      <c r="D49" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20" t="s">
+      <c r="E49" s="14"/>
+      <c r="F49" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="G49" s="20" t="s">
+      <c r="G49" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="H49" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="I49" s="21"/>
-    </row>
-    <row r="50" spans="2:9">
+      <c r="H49" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I49" s="15"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
         <v>83</v>
       </c>
@@ -1970,7 +1967,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="2:9">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
         <v>86</v>
       </c>
@@ -1991,7 +1988,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="2:9">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
         <v>87</v>
       </c>
@@ -2012,7 +2009,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="2:9">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
         <v>17</v>
       </c>
@@ -2033,7 +2030,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="2:9">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
         <v>22</v>
       </c>
@@ -2054,7 +2051,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="2:9">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
         <v>89</v>
       </c>
@@ -2075,18 +2072,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="57" spans="2:9" ht="50.1" customHeight="1">
-      <c r="B57" s="13" t="s">
+    <row r="57" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C57" s="13"/>
-      <c r="D57" s="13"/>
-      <c r="E57" s="13"/>
-      <c r="F57" s="13"/>
-      <c r="G57" s="13"/>
-      <c r="H57" s="13"/>
-    </row>
-    <row r="58" spans="2:9" s="1" customFormat="1">
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="19"/>
+    </row>
+    <row r="58" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
         <v>6</v>
       </c>
@@ -2109,7 +2106,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="2:9">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
         <v>91</v>
       </c>
@@ -2130,7 +2127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:9">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
         <v>94</v>
       </c>
@@ -2151,7 +2148,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="2:9">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
         <v>72</v>
       </c>
@@ -2172,18 +2169,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="2:9" ht="50.1" customHeight="1">
-      <c r="B63" s="14" t="s">
+    <row r="63" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="C63" s="15"/>
-      <c r="D63" s="15"/>
-      <c r="E63" s="15"/>
-      <c r="F63" s="15"/>
-      <c r="G63" s="15"/>
-      <c r="H63" s="16"/>
-    </row>
-    <row r="64" spans="2:9" s="1" customFormat="1">
+      <c r="C63" s="21"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="21"/>
+      <c r="G63" s="21"/>
+      <c r="H63" s="22"/>
+    </row>
+    <row r="64" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
         <v>6</v>
       </c>
@@ -2206,7 +2203,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="2:9">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
         <v>99</v>
       </c>
@@ -2227,7 +2224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="2:9">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
         <v>101</v>
       </c>
@@ -2248,7 +2245,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="67" spans="2:9">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="3" t="s">
         <v>72</v>
       </c>
@@ -2269,7 +2266,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="2:9" ht="15.95" customHeight="1">
+    <row r="68" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
         <v>105</v>
       </c>
@@ -2290,7 +2287,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="2:9" ht="15.95" customHeight="1">
+    <row r="69" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="s">
         <v>108</v>
       </c>
@@ -2309,37 +2306,37 @@
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="2:9" ht="15.95" customHeight="1">
-      <c r="B70" s="20" t="s">
+    <row r="70" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="C70" s="20" t="s">
+      <c r="C70" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="D70" s="20"/>
-      <c r="E70" s="20"/>
-      <c r="F70" s="20" t="s">
+      <c r="D70" s="14"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="G70" s="20">
+      <c r="G70" s="14">
         <v>300</v>
       </c>
-      <c r="H70" s="20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="72" spans="2:9" ht="50.1" customHeight="1">
-      <c r="B72" s="13" t="s">
+      <c r="H70" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="72" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="C72" s="13"/>
-      <c r="D72" s="13"/>
-      <c r="E72" s="13"/>
-      <c r="F72" s="13"/>
-      <c r="G72" s="13"/>
-      <c r="H72" s="13"/>
-    </row>
-    <row r="73" spans="2:9" s="1" customFormat="1">
+      <c r="C72" s="19"/>
+      <c r="D72" s="19"/>
+      <c r="E72" s="19"/>
+      <c r="F72" s="19"/>
+      <c r="G72" s="19"/>
+      <c r="H72" s="19"/>
+    </row>
+    <row r="73" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="2" t="s">
         <v>6</v>
       </c>
@@ -2362,7 +2359,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="2:9" s="1" customFormat="1">
+    <row r="74" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="6" t="s">
         <v>115</v>
       </c>
@@ -2383,7 +2380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="2:9">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="3" t="s">
         <v>99</v>
       </c>
@@ -2404,7 +2401,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="2:9">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="s">
         <v>118</v>
       </c>
@@ -2425,27 +2422,27 @@
         <v>21</v>
       </c>
     </row>
-    <row r="77" spans="2:9">
-      <c r="B77" s="20" t="s">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B77" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="C77" s="20" t="s">
+      <c r="C77" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="D77" s="20"/>
-      <c r="E77" s="20"/>
-      <c r="F77" s="20" t="s">
+      <c r="D77" s="14"/>
+      <c r="E77" s="14"/>
+      <c r="F77" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="G77" s="20">
+      <c r="G77" s="14">
         <v>300</v>
       </c>
-      <c r="H77" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="I77" s="23"/>
-    </row>
-    <row r="78" spans="2:9">
+      <c r="H77" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I77" s="17"/>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="s">
         <v>123</v>
       </c>
@@ -2466,18 +2463,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="2:9" ht="50.1" customHeight="1">
-      <c r="B80" s="13" t="s">
+    <row r="80" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="C80" s="13"/>
-      <c r="D80" s="13"/>
-      <c r="E80" s="13"/>
-      <c r="F80" s="13"/>
-      <c r="G80" s="13"/>
-      <c r="H80" s="13"/>
-    </row>
-    <row r="81" spans="2:9" s="1" customFormat="1">
+      <c r="C80" s="19"/>
+      <c r="D80" s="19"/>
+      <c r="E80" s="19"/>
+      <c r="F80" s="19"/>
+      <c r="G80" s="19"/>
+      <c r="H80" s="19"/>
+    </row>
+    <row r="81" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
         <v>6</v>
       </c>
@@ -2500,7 +2497,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="2:9">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="s">
         <v>105</v>
       </c>
@@ -2521,7 +2518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="2:9">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="3" t="s">
         <v>129</v>
       </c>
@@ -2542,29 +2539,29 @@
         <v>21</v>
       </c>
     </row>
-    <row r="84" spans="2:9">
-      <c r="B84" s="20" t="s">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B84" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="C84" s="20" t="s">
+      <c r="C84" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="D84" s="20"/>
-      <c r="E84" s="20">
+      <c r="D84" s="14"/>
+      <c r="E84" s="14">
         <v>6</v>
       </c>
-      <c r="F84" s="20" t="s">
+      <c r="F84" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="G84" s="22" t="s">
+      <c r="G84" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="H84" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="I84" s="21"/>
-    </row>
-    <row r="85" spans="2:9">
+      <c r="H84" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I84" s="15"/>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="3" t="s">
         <v>135</v>
       </c>
@@ -2585,18 +2582,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="87" spans="2:9" ht="50.1" customHeight="1">
-      <c r="B87" s="13" t="s">
+    <row r="87" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="C87" s="13"/>
-      <c r="D87" s="13"/>
-      <c r="E87" s="13"/>
-      <c r="F87" s="13"/>
-      <c r="G87" s="13"/>
-      <c r="H87" s="13"/>
-    </row>
-    <row r="88" spans="2:9" s="1" customFormat="1">
+      <c r="C87" s="19"/>
+      <c r="D87" s="19"/>
+      <c r="E87" s="19"/>
+      <c r="F87" s="19"/>
+      <c r="G87" s="19"/>
+      <c r="H87" s="19"/>
+    </row>
+    <row r="88" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
         <v>6</v>
       </c>
@@ -2619,7 +2616,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="2:9">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="3" t="s">
         <v>139</v>
       </c>
@@ -2640,7 +2637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="2:9">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="3" t="s">
         <v>54</v>
       </c>
@@ -2659,7 +2656,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="2:9">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="3" t="s">
         <v>142</v>
       </c>
@@ -2680,7 +2677,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="92" spans="2:9">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="3" t="s">
         <v>146</v>
       </c>
@@ -2701,7 +2698,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="93" spans="2:9">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" s="3" t="s">
         <v>149</v>
       </c>
@@ -2720,7 +2717,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="94" spans="2:9">
+    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" s="3" t="s">
         <v>105</v>
       </c>
@@ -2741,18 +2738,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B87:H87"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="B63:H63"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="B72:H72"/>
     <mergeCell ref="B80:H80"/>
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="B6:H6"/>
     <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B87:H87"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="B63:H63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2760,18 +2757,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2960,13 +2957,37 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{718FCF40-0A5E-4007-8F6E-B9865DED1CAB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{160433BB-9D03-4DD4-9AC5-6D924538AFC5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{160433BB-9D03-4DD4-9AC5-6D924538AFC5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{718FCF40-0A5E-4007-8F6E-B9865DED1CAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5079184-C4BA-4DAC-B1BD-DF2D74DA512D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5079184-C4BA-4DAC-B1BD-DF2D74DA512D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9d58e15a-28f4-4c04-a7e2-ae26ac84ad24"/>
+    <ds:schemaRef ds:uri="9784e1bf-9cce-483b-b54d-e9a62e69548b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>